<commit_message>
ADDED - BLog Pt2
</commit_message>
<xml_diff>
--- a/data/asg/social/social_diversidad_inclusion.xlsx
+++ b/data/asg/social/social_diversidad_inclusion.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Distribución de personal por tipo de puesto</t>
   </si>
@@ -33,25 +33,25 @@
     <t xml:space="preserve">Gerencias</t>
   </si>
   <si>
-    <t xml:space="preserve">Direccón</t>
-  </si>
-  <si>
-    <t xml:space="preserve">102-46.4%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15-62.61%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-28.6%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">118-53.6%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9-37.5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5-71.4%</t>
+    <t xml:space="preserve">Dirección</t>
+  </si>
+  <si>
+    <t xml:space="preserve">131 – 53%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 – 61%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 – 40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">118 – 47%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 – 39%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 – 60%</t>
   </si>
   <si>
     <t xml:space="preserve">Junta Directiva por género</t>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t xml:space="preserve">Nuevas contrataciones por género</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46 – 48%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 – 52%</t>
   </si>
 </sst>
 </file>
@@ -144,20 +150,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -353,54 +363,54 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>119</v>
+      <c r="D3" s="1" t="n">
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>132</v>
+      <c r="D4" s="1" t="n">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -427,20 +437,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>11</v>
       </c>
     </row>
@@ -460,29 +470,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>11</v>
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>